<commit_message>
Custom Question Generation Code
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata/TestData.xlsx
+++ b/src/test/java/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aptitudo\Aptitudo_Auto\src\test\java\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA60B5A-450F-49CF-A102-C5B4BE218CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0AAEF5-EBCE-4265-8557-9AE81149D246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{F7F1F9E0-F06A-4449-B18B-97F7046185DE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>admin</t>
   </si>
@@ -104,6 +104,166 @@
   </si>
   <si>
     <t>Java</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Write a function that takes a list of integers and returns the second largest number in the list. If there is no second largest (e.g., all numbers are equal), return None.</t>
+  </si>
+  <si>
+    <t>The list must contain at least two integers</t>
+  </si>
+  <si>
+    <t>The integers can be negative or positive</t>
+  </si>
+  <si>
+    <t>Do not use built-in sort functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input: [10, 20, 4, 45, 99] </t>
+  </si>
+  <si>
+    <t>Output: 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input: [5, 5, 5]  </t>
+  </si>
+  <si>
+    <t>Output: null</t>
+  </si>
+  <si>
+    <t>The largest number is 99
+The second largest is 45</t>
+  </si>
+  <si>
+    <t>All numbers are the same, so there is no distinct second largest</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>Which of the following is NOT a responsibility of a QA Lead?</t>
+  </si>
+  <si>
+    <t>Defining the test strategy</t>
+  </si>
+  <si>
+    <t>Assigning tasks to team members</t>
+  </si>
+  <si>
+    <t>Writing production code</t>
+  </si>
+  <si>
+    <t>Reporting test metrics to stakeholders</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>What is the primary purpose of a test plan?</t>
+  </si>
+  <si>
+    <t>To list all developers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To define the code review process</t>
+  </si>
+  <si>
+    <t>To outline testing scope, strategy, and schedule</t>
+  </si>
+  <si>
+    <t>To assign test cases to customers</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>In Agile, the QA Lead should primarily focus on:</t>
+  </si>
+  <si>
+    <t>Writing all test cases alone</t>
+  </si>
+  <si>
+    <t>Ensuring manual testing is eliminated</t>
+  </si>
+  <si>
+    <t>Facilitating continuous testing and team collaboration</t>
+  </si>
+  <si>
+    <t>Blocking releases until full test coverage is achieved</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>Which testing type is best suited for identifying system bottlenecks?</t>
+  </si>
+  <si>
+    <t>Smoke Testing</t>
+  </si>
+  <si>
+    <t>Regression Testing</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Usability Testing</t>
+  </si>
+  <si>
+    <t>A defect is rejected by a developer due to “Works as Designed.” What should the QA Lead do next?</t>
+  </si>
+  <si>
+    <t>Escalate immediately to the client</t>
+  </si>
+  <si>
+    <t>Close the defect</t>
+  </si>
+  <si>
+    <t>Re-open with screenshots only</t>
+  </si>
+  <si>
+    <t>Review the requirement and facilitate a discussion</t>
+  </si>
+  <si>
+    <t>File Upload</t>
+  </si>
+  <si>
+    <t>Upload your CV with Cover Letter</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>Introduce yourself</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>Describe the key responsibilities and skills required for a Software Quality Assurance (SQA) Lead. How does an SQA Lead contribute to the success of a software development project?</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>How do you ensure the quality of a software product?</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>What is your approach to managing a QA team?</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>How do you handle critical bugs during a release cycle?</t>
   </si>
 </sst>
 </file>
@@ -119,12 +279,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,13 +305,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,21 +653,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4C4AE3-27A2-4EEF-87DB-CE482C31C29F}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.28515625" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="83.28515625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="330" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -511,109 +683,343 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>90</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>120</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>70</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2">
+        <v>300</v>
+      </c>
+      <c r="C14" s="2">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="2">
+        <v>200</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2">
+        <v>200</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="2">
+        <v>200</v>
+      </c>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test from AI
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata/TestData.xlsx
+++ b/src/test/java/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aptitudo\Aptitudo_Auto\src\test\java\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0AAEF5-EBCE-4265-8557-9AE81149D246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A562AABD-7A72-4980-8AAF-D6DFE8B615A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{F7F1F9E0-F06A-4449-B18B-97F7046185DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F7F1F9E0-F06A-4449-B18B-97F7046185DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>admin</t>
   </si>
@@ -265,18 +265,30 @@
   <si>
     <t>How do you handle critical bugs during a release cycle?</t>
   </si>
+  <si>
+    <t>wert</t>
+  </si>
+  <si>
+    <t>test-code-004</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF111827"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -305,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -316,6 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,10 +666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4C4AE3-27A2-4EEF-87DB-CE482C31C29F}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +845,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -854,8 +867,11 @@
       <c r="G7" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -876,6 +892,9 @@
       </c>
       <c r="G8" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -900,6 +919,9 @@
       <c r="G9" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -923,6 +945,9 @@
       <c r="G10" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -946,6 +971,9 @@
       <c r="G11" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="H11" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1022,7 +1050,28 @@
         <v>72</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aptitudo Question Generation and Send Invitation
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata/TestData.xlsx
+++ b/src/test/java/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aptitudo\Aptitudo_Auto\src\test\java\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A562AABD-7A72-4980-8AAF-D6DFE8B615A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4BF26A-173F-4AA1-A94A-F71D6EB1CD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F7F1F9E0-F06A-4449-B18B-97F7046185DE}"/>
+    <workbookView xWindow="9375" yWindow="1335" windowWidth="21030" windowHeight="11070" activeTab="1" xr2:uid="{F7F1F9E0-F06A-4449-B18B-97F7046185DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>admin</t>
   </si>
@@ -254,29 +254,29 @@
     <t>How do you ensure the quality of a software product?</t>
   </si>
   <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>What is your approach to managing a QA team?</t>
-  </si>
-  <si>
-    <t>S3</t>
-  </si>
-  <si>
-    <t>How do you handle critical bugs during a release cycle?</t>
-  </si>
-  <si>
-    <t>wert</t>
-  </si>
-  <si>
-    <t>test-code-004</t>
+    <t>Tamima</t>
+  </si>
+  <si>
+    <t>Tarin</t>
+  </si>
+  <si>
+    <t>tarin.aiub@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nourin </t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>nourinahmed.nuba@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +287,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF111827"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -314,10 +328,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -329,8 +344,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -666,17 +692,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4C4AE3-27A2-4EEF-87DB-CE482C31C29F}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="83.28515625" style="2" customWidth="1"/>
     <col min="6" max="7" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -1022,56 +1048,41 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="2">
-        <v>200</v>
-      </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="2">
-        <v>200</v>
-      </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
+    </row>
+    <row r="17" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="B17" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="C17" s="8" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{FC8B367F-7DFA-4B4D-AC96-2A9054DD9D6B}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{48444704-868C-4346-8115-5174BFD940AF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>